<commit_message>
correção das notas do fórum  para matc65 em 2021.2
</commit_message>
<xml_diff>
--- a/build/ensino/2022/08/segundo-semestre-de-2022/mes-10-dia-16-ava-matc65.xlsx
+++ b/build/ensino/2022/08/segundo-semestre-de-2022/mes-10-dia-16-ava-matc65.xlsx
@@ -455,22 +455,22 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -493,16 +493,16 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -528,13 +528,13 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -595,10 +595,10 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -606,10 +606,10 @@
         <v>220215074</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -627,10 +627,10 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -673,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -688,13 +688,13 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -708,13 +708,13 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -723,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -737,16 +737,16 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -755,10 +755,10 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -787,10 +787,10 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -798,16 +798,16 @@
         <v>220120072</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -819,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -833,16 +833,16 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -851,10 +851,10 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -883,10 +883,10 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -915,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -932,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -947,10 +947,10 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -958,10 +958,10 @@
         <v>218118315</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -970,19 +970,19 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1028,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1043,10 +1043,10 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1060,13 +1060,13 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1075,10 +1075,10 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1086,31 +1086,31 @@
         <v>219118768</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1121,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1139,10 +1139,10 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1150,10 +1150,10 @@
         <v>220215670</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1171,10 +1171,10 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1185,28 +1185,28 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1226,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1235,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1249,16 +1249,16 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1267,10 +1267,10 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1316,25 +1316,25 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1377,13 +1377,13 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1392,13 +1392,13 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1438,10 +1438,10 @@
         <v>220117289</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1459,10 +1459,10 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1470,10 +1470,10 @@
         <v>219218353</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1485,16 +1485,16 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1523,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1572,25 +1572,25 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1598,7 +1598,7 @@
         <v>219119774</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1607,22 +1607,22 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1636,25 +1636,25 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1712,13 +1712,13 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1741,16 +1741,16 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1758,31 +1758,31 @@
         <v>221117685</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1854,10 +1854,10 @@
         <v>220217141</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1866,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1875,10 +1875,10 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1936,13 +1936,13 @@
         <v>0</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1965,16 +1965,16 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>